<commit_message>
OO-3074: remove the description from the import template
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="0" windowWidth="36080" windowHeight="30860" tabRatio="500"/>
+    <workbookView xWindow="6280" yWindow="1720" windowWidth="28540" windowHeight="21520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="99">
   <si>
     <t>Typ</t>
   </si>
@@ -33,9 +33,6 @@
     <t xml:space="preserve">Wird in Navigation angezeigt. Entspricht dem Thema der Frage. </t>
   </si>
   <si>
-    <t>Optionale Beschreibung / Einführungstext der zwischen dem Titel und dem eigentlichen Lückentext erscheint. Worum geht es in diesem Frageitem?</t>
-  </si>
-  <si>
     <t>Die maximal zu erreichende Punktzahl</t>
   </si>
   <si>
@@ -78,12 +75,6 @@
     <t>Fussball: Austragungsort</t>
   </si>
   <si>
-    <t>Die Fussball WM wird alle vier Jahre von einem anderen Land ausgerichtet.</t>
-  </si>
-  <si>
-    <t>Optionale Beschreibung / Einführungstext der zwischen dem Titel und der eigentlichen Frage erscheint. Worum geht es in dieser Frage?</t>
-  </si>
-  <si>
     <t>In welchen Ländern wurde zwischen dem Jahr 2000 und 2015 eine Fussball Weltmeisterschaft ausgetragen?</t>
   </si>
   <si>
@@ -147,9 +138,6 @@
     <t>Fussball: Gewinner</t>
   </si>
   <si>
-    <t>Im Jahr 1982 wurde die WM in Spanien ausgetragen.</t>
-  </si>
-  <si>
     <t>Spanien</t>
   </si>
   <si>
@@ -204,9 +192,6 @@
     <t>Editor Version</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -216,9 +201,6 @@
     <t>Points</t>
   </si>
   <si>
-    <t>Eine lange Beschreibung</t>
-  </si>
-  <si>
     <t>Englisch Wortschatz</t>
   </si>
   <si>
@@ -328,9 +310,6 @@
   </si>
   <si>
     <t>Fussball: Weltmeister</t>
-  </si>
-  <si>
-    <t>Prüfen Sie die Weltmeiser kennen</t>
   </si>
   <si>
     <t>Uruguay</t>
@@ -915,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -932,16 +911,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -949,19 +928,19 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="12" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -971,290 +950,292 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4">
       <c r="A5" s="6" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>66</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="7"/>
       <c r="D6" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30">
       <c r="A11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>70</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B11" s="8"/>
       <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B13" s="8">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B14" s="8">
-        <v>0.6</v>
+        <v>-0.33</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B15" s="8">
-        <v>-0.33</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30">
       <c r="A17" s="6" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45">
       <c r="A18" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>95</v>
+        <v>56</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>73</v>
+      <c r="A20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="4" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="7">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30">
+      <c r="A22" s="5">
+        <v>1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="D22" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30">
-      <c r="A23" s="5">
-        <v>1</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45">
+    </row>
+    <row r="24" spans="1:4">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="4"/>
+      <c r="A25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="4" t="s">
-        <v>89</v>
-      </c>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>11</v>
+        <v>59</v>
+      </c>
+      <c r="B27" s="7">
+        <v>5</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="8"/>
+      <c r="A28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C28" s="7"/>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="7">
-        <v>5</v>
-      </c>
-      <c r="C29" s="7"/>
+      <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="4"/>
@@ -1263,17 +1244,15 @@
       <c r="A31" s="5">
         <v>1</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>15</v>
@@ -1287,13 +1266,13 @@
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>16</v>
@@ -1302,119 +1281,121 @@
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="5">
-        <v>1</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B35" s="10"/>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="10"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="B37" s="10"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="B38" s="10"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D38" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45">
       <c r="A39" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>38</v>
+        <v>65</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>18</v>
+        <v>59</v>
+      </c>
+      <c r="B40" s="7">
+        <v>3</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30">
-      <c r="A41" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="5">
+        <v>1</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45">
-      <c r="A42" s="5" t="s">
-        <v>71</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="5">
+        <v>1</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="7">
-        <v>3</v>
+      <c r="A43" s="5">
+        <v>1</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1422,123 +1403,123 @@
         <v>-1</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="5">
-        <v>-1</v>
-      </c>
-      <c r="B48" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30">
+      <c r="B48" s="10"/>
+      <c r="D48" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="5">
-        <v>-1</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="B49" s="10"/>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="5">
-        <v>-1</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30">
-      <c r="B51" s="10"/>
-      <c r="D51" s="4" t="s">
-        <v>32</v>
+      <c r="B50" s="10"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="B52" s="10"/>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="B53" s="10"/>
-      <c r="D53" s="4"/>
+      <c r="A52" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30">
+      <c r="A53" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="7">
+        <v>1</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="5">
         <v>0</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B55" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="5">
+        <v>0</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="5">
+        <v>0</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="5">
+        <v>0</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D54" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="8" t="s">
+      <c r="D58" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="30">
-      <c r="A57" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="7">
-        <v>1</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1546,10 +1527,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1557,158 +1538,103 @@
         <v>0</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30">
+      <c r="D62" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="5">
+      <c r="B64" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="45">
+      <c r="A66" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" s="7">
         <v>1</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="5">
-        <v>0</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="5">
-        <v>0</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="30">
-      <c r="D66" s="4" t="s">
-        <v>32</v>
+      <c r="D67" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="5" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="30">
-      <c r="A70" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>103</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="5" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="7">
-        <v>1</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OO-3090	: add hint and correct solution to the field the CSV importer can manage
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="1720" windowWidth="28540" windowHeight="21520" tabRatio="500"/>
+    <workbookView xWindow="1660" yWindow="1300" windowWidth="28540" windowHeight="21520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="104">
   <si>
     <t>Typ</t>
   </si>
@@ -316,6 +316,21 @@
   </si>
   <si>
     <t>Die folgenden Länder haben die Fussball Weltmeistertitel bereits mehr als einmal gewonnen.</t>
+  </si>
+  <si>
+    <t>Information: alle optionalen Felder aus dem Type FIB können auch bei den anderen Fragetypen hinzugefügt werden. Fügen Sie dazu unter Titel die entsprechenden Zeilen ein.</t>
+  </si>
+  <si>
+    <t>Hint</t>
+  </si>
+  <si>
+    <t>Correct solution</t>
+  </si>
+  <si>
+    <t>Antworten Januar und Februar sind korrekt</t>
+  </si>
+  <si>
+    <t>Denken Sie an die Theorie von Max Mustermann.</t>
   </si>
 </sst>
 </file>
@@ -485,7 +500,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -521,6 +536,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -894,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -924,330 +942,326 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="14" customHeight="1">
+      <c r="A3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="12" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="8"/>
       <c r="C6" s="7"/>
       <c r="D6" s="4" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="7"/>
       <c r="D8" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30">
       <c r="A11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="8"/>
+        <v>48</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="8">
-        <v>0.55000000000000004</v>
+        <v>49</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0.6</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="7"/>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="8">
-        <v>-0.33</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="8">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>66</v>
+        <v>53</v>
+      </c>
+      <c r="B16" s="8">
+        <v>-0.33</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>88</v>
+        <v>54</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30">
       <c r="A19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>67</v>
+        <v>100</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="7">
-        <v>1</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30">
+      <c r="A20" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>6</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30">
+      <c r="A21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30">
-      <c r="A22" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45">
+      <c r="A22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="7">
         <v>1</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="4"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30">
+      <c r="A26" s="5">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="7">
-        <v>5</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="5">
-        <v>1</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="5" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="5">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="A31" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="7">
+        <v>5</v>
+      </c>
+      <c r="C31" s="7"/>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4">
@@ -1255,7 +1269,7 @@
         <v>5</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="4"/>
@@ -1264,7 +1278,9 @@
       <c r="A33" s="5">
         <v>1</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C33" s="7" t="s">
         <v>13</v>
       </c>
@@ -1275,251 +1291,247 @@
         <v>5</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="B35" s="10"/>
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="B36" s="10"/>
+      <c r="A36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="7"/>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>35</v>
-      </c>
+      <c r="A37" s="5">
+        <v>1</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="B39" s="10"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="B40" s="10"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B42" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45">
-      <c r="A39" s="5" t="s">
+    <row r="43" spans="1:4" ht="45">
+      <c r="A43" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B43" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="5" t="s">
+    <row r="44" spans="1:4">
+      <c r="A44" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B44" s="7">
         <v>3</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="5">
-        <v>1</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="5">
-        <v>1</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="5">
-        <v>1</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="5">
-        <v>-1</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="5">
+        <v>1</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="5">
         <v>-1</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30">
-      <c r="B48" s="10"/>
-      <c r="D48" s="4" t="s">
+    <row r="52" spans="1:4" ht="30">
+      <c r="B52" s="10"/>
+      <c r="D52" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="B49" s="10"/>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="B50" s="10"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="5" t="s">
+    <row r="53" spans="1:4">
+      <c r="B53" s="10"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="B54" s="10"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D55" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="5" t="s">
+    <row r="56" spans="1:4">
+      <c r="A56" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B56" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="30">
-      <c r="A53" s="5" t="s">
+    <row r="57" spans="1:4" ht="30">
+      <c r="A57" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="5" t="s">
+    <row r="58" spans="1:4">
+      <c r="A58" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B58" s="7">
         <v>1</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="5">
-        <v>0</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="5">
-        <v>0</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="5">
-        <v>0</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="5">
-        <v>0</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1527,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>42</v>
@@ -1538,106 +1550,153 @@
         <v>0</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30">
+    <row r="62" spans="1:4">
+      <c r="A62" s="5">
+        <v>0</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="D62" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="5">
+        <v>1</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="5">
+        <v>0</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="5">
+        <v>0</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="30">
+      <c r="D66" s="4" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="45">
-      <c r="A66" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" s="7">
-        <v>1</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>95</v>
+        <v>0</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="5" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="45">
       <c r="A70" s="5" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="7">
+        <v>1</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B72" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
OO-3174: CSV import of essay and match in QTI 2.1
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1300" windowWidth="28540" windowHeight="21520" tabRatio="500"/>
+    <workbookView xWindow="7940" yWindow="4200" windowWidth="30760" windowHeight="21480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="122">
   <si>
     <t>Typ</t>
   </si>
@@ -331,6 +339,60 @@
   </si>
   <si>
     <t>Denken Sie an die Theorie von Max Mustermann.</t>
+  </si>
+  <si>
+    <t>ESSAY</t>
+  </si>
+  <si>
+    <t>Fussball: Spieler</t>
+  </si>
+  <si>
+    <t>Wer ist der beste Spieler aller Zeit?</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>MATRIX</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Hauptstädte Europas</t>
+  </si>
+  <si>
+    <t>Drag&amp;drop</t>
+  </si>
+  <si>
+    <t>Hauptstädte Afrika</t>
+  </si>
+  <si>
+    <t>Algerien</t>
+  </si>
+  <si>
+    <t>Algier</t>
+  </si>
+  <si>
+    <t>Kenia</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nairobi</t>
+  </si>
+  <si>
+    <t>Windhoek</t>
   </si>
 </sst>
 </file>
@@ -543,50 +605,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="41">
-    <cellStyle name="Ausgabe" xfId="16" builtinId="21"/>
-    <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
-    <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Sortie" xfId="16" builtinId="21"/>
+    <cellStyle name="Texte explicatif" xfId="1" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -912,13 +979,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
@@ -927,7 +994,7 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -941,13 +1008,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="14" customHeight="1">
+    <row r="3" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>99</v>
       </c>
@@ -955,10 +1022,10 @@
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -970,7 +1037,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
@@ -982,7 +1049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>44</v>
       </c>
@@ -994,7 +1061,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>45</v>
       </c>
@@ -1004,7 +1071,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
@@ -1016,7 +1083,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>47</v>
       </c>
@@ -1028,7 +1095,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>48</v>
       </c>
@@ -1040,7 +1107,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
@@ -1052,7 +1119,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>50</v>
       </c>
@@ -1062,7 +1129,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
@@ -1074,7 +1141,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
@@ -1086,7 +1153,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>53</v>
       </c>
@@ -1098,7 +1165,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
@@ -1110,7 +1177,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>55</v>
       </c>
@@ -1122,7 +1189,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>100</v>
       </c>
@@ -1134,7 +1201,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>101</v>
       </c>
@@ -1146,7 +1213,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30">
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>86</v>
       </c>
@@ -1158,7 +1225,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
+    <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>87</v>
       </c>
@@ -1170,7 +1237,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>56</v>
       </c>
@@ -1182,7 +1249,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>59</v>
       </c>
@@ -1194,7 +1261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -1206,7 +1273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>1</v>
       </c>
@@ -1220,19 +1287,19 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45">
+    <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>58</v>
       </c>
@@ -1244,7 +1311,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>57</v>
       </c>
@@ -1254,7 +1321,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>59</v>
       </c>
@@ -1264,7 +1331,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
@@ -1274,7 +1341,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>1</v>
       </c>
@@ -1286,7 +1353,7 @@
       </c>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -1296,7 +1363,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>1</v>
       </c>
@@ -1306,7 +1373,7 @@
       </c>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
@@ -1316,7 +1383,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>1</v>
       </c>
@@ -1326,7 +1393,7 @@
       </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
@@ -1336,15 +1403,15 @@
       <c r="C38" s="7"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="10"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="10"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>57</v>
       </c>
@@ -1366,7 +1433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45">
+    <row r="43" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>65</v>
       </c>
@@ -1377,7 +1444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>59</v>
       </c>
@@ -1388,7 +1455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>1</v>
       </c>
@@ -1399,7 +1466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>1</v>
       </c>
@@ -1410,7 +1477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>1</v>
       </c>
@@ -1421,7 +1488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>-1</v>
       </c>
@@ -1432,7 +1499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>-1</v>
       </c>
@@ -1443,7 +1510,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>-1</v>
       </c>
@@ -1454,7 +1521,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>-1</v>
       </c>
@@ -1465,21 +1532,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30">
+    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B52" s="10"/>
       <c r="D52" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53" s="10"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B54" s="10"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>0</v>
       </c>
@@ -1490,7 +1557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>57</v>
       </c>
@@ -1501,7 +1568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30">
+    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>65</v>
       </c>
@@ -1512,7 +1579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>59</v>
       </c>
@@ -1523,7 +1590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <v>0</v>
       </c>
@@ -1534,7 +1601,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>0</v>
       </c>
@@ -1545,7 +1612,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>0</v>
       </c>
@@ -1556,7 +1623,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>0</v>
       </c>
@@ -1567,7 +1634,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>1</v>
       </c>
@@ -1578,7 +1645,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>0</v>
       </c>
@@ -1589,7 +1656,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>0</v>
       </c>
@@ -1600,12 +1667,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="30">
+    <row r="66" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="D66" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>0</v>
       </c>
@@ -1616,7 +1683,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>57</v>
       </c>
@@ -1627,7 +1694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="45">
+    <row r="70" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>65</v>
       </c>
@@ -1638,7 +1705,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>59</v>
       </c>
@@ -1649,7 +1716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>93</v>
       </c>
@@ -1660,7 +1727,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>94</v>
       </c>
@@ -1671,7 +1738,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>94</v>
       </c>
@@ -1682,7 +1749,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>93</v>
       </c>
@@ -1691,6 +1758,226 @@
       </c>
       <c r="D75" s="4" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B82" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B83" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B89" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="5"/>
+      <c r="B90" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B91" s="7">
+        <v>1</v>
+      </c>
+      <c r="C91" s="7">
+        <v>0</v>
+      </c>
+      <c r="D91" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B92" s="7">
+        <v>0</v>
+      </c>
+      <c r="C92" s="7">
+        <v>0</v>
+      </c>
+      <c r="D92" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B93" s="7">
+        <v>0</v>
+      </c>
+      <c r="C93" s="7">
+        <v>1</v>
+      </c>
+      <c r="D93" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B99" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="5"/>
+      <c r="B100" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B101" s="7">
+        <v>0</v>
+      </c>
+      <c r="C101" s="7">
+        <v>1</v>
+      </c>
+      <c r="D101" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B102" s="7">
+        <v>0</v>
+      </c>
+      <c r="C102" s="7">
+        <v>0</v>
+      </c>
+      <c r="D102" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B103" s="7">
+        <v>1</v>
+      </c>
+      <c r="C103" s="7">
+        <v>0</v>
+      </c>
+      <c r="D103" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1699,10 +1986,5 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OO-3220: true/false question type based on the matchInteraction with specific behavior
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Developer/Work/ws_alternative/OpenOLAT/src/main/resources/org/olat/ims/qti21/questionimport/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="4200" windowWidth="30760" windowHeight="21480" tabRatio="500"/>
+    <workbookView xWindow="5080" yWindow="460" windowWidth="28320" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="130">
   <si>
     <t>Typ</t>
   </si>
@@ -393,6 +393,30 @@
   </si>
   <si>
     <t>Windhoek</t>
+  </si>
+  <si>
+    <t>Truefalse</t>
+  </si>
+  <si>
+    <t>Hauptstädte Europa</t>
+  </si>
+  <si>
+    <t>Unanswered</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Wrong</t>
+  </si>
+  <si>
+    <t>Paris ist in Frankreich</t>
+  </si>
+  <si>
+    <t>Bern ist in Schweiz</t>
+  </si>
+  <si>
+    <t>Stockholm ist in Danemark</t>
   </si>
 </sst>
 </file>
@@ -979,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1980,6 +2004,92 @@
         <v>0</v>
       </c>
     </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B109" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="5"/>
+      <c r="B110" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B111" s="7">
+        <v>0</v>
+      </c>
+      <c r="C111" s="7">
+        <v>1</v>
+      </c>
+      <c r="D111" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B112" s="7">
+        <v>0</v>
+      </c>
+      <c r="C112" s="7">
+        <v>1</v>
+      </c>
+      <c r="D112" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B113" s="7">
+        <v>0</v>
+      </c>
+      <c r="C113" s="7">
+        <v>0</v>
+      </c>
+      <c r="D113" s="7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:D3"/>

</xml_diff>

<commit_message>
OO-3536: add topic to the imported metadata in question pool
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Developer/Work/ws_alternative/OpenOLAT/src/main/resources/org/olat/ims/qti21/questionimport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF45A0EF-AF9E-224E-B060-D1C5DC7DBEAA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="460" windowWidth="28320" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="5080" yWindow="460" windowWidth="28320" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="133">
   <si>
     <t>Typ</t>
   </si>
@@ -417,12 +418,21 @@
   </si>
   <si>
     <t>Stockholm ist in Danemark</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Grundwortschatz</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Thema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -676,6 +686,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1002,11 +1015,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D113"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:D113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,162 +1088,162 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="C8" s="7"/>
       <c r="D8" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>61</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="8">
-        <v>0.55000000000000004</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="7"/>
       <c r="D14" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="8">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="8">
-        <v>-0.33</v>
+        <v>0.6</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="8">
-        <v>1</v>
+        <v>-0.33</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="4" t="s">
@@ -1239,196 +1252,204 @@
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>67</v>
+        <v>87</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="4" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="7">
-        <v>1</v>
+      <c r="A24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="4" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>6</v>
+        <v>59</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
-        <v>1</v>
-      </c>
-      <c r="B26" s="7" t="s">
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>1</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>10</v>
+        <v>58</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="7">
-        <v>5</v>
+        <v>57</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="7">
         <v>5</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
-        <v>1</v>
+      <c r="A33" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
-        <v>1</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="7"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>1</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
-        <v>1</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="7"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>1</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B39" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="10"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1436,58 +1457,51 @@
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>35</v>
-      </c>
+      <c r="B41" s="10"/>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B43" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B44" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B45" s="7">
         <v>3</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="5">
-        <v>1</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1495,7 +1509,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>21</v>
@@ -1506,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>21</v>
@@ -1514,13 +1528,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1528,7 +1542,7 @@
         <v>-1</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>25</v>
@@ -1539,7 +1553,7 @@
         <v>-1</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>25</v>
@@ -1550,79 +1564,79 @@
         <v>-1</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B52" s="10"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D52" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B53" s="10"/>
+      <c r="D53" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="10"/>
-      <c r="D53" s="4"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B54" s="10"/>
       <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="B55" s="10"/>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="7">
-        <v>1</v>
-      </c>
-      <c r="D58" s="4" t="s">
+      <c r="B59" s="7">
+        <v>1</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="5">
-        <v>0</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1630,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>42</v>
@@ -1641,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>42</v>
@@ -1652,7 +1666,7 @@
         <v>0</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>42</v>
@@ -1660,24 +1674,24 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1685,81 +1699,81 @@
         <v>0</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>0</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D66" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="D67" s="4" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B70" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D71" s="4" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B71" s="7">
-        <v>1</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>20</v>
+        <v>59</v>
+      </c>
+      <c r="B72" s="7">
+        <v>1</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>95</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1767,7 +1781,7 @@
         <v>94</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>42</v>
@@ -1775,82 +1789,85 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B76" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B81" s="7">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="B82" s="7">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B83" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B84" s="7">
         <v>2000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>113</v>
+        <v>0</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>113</v>
@@ -1858,85 +1875,85 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="5"/>
-      <c r="B90" s="11" t="s">
+      <c r="B90" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="5"/>
+      <c r="B91" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C91" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D90" s="11" t="s">
+      <c r="D91" s="11" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B91" s="7">
-        <v>1</v>
-      </c>
-      <c r="C91" s="7">
-        <v>0</v>
-      </c>
-      <c r="D91" s="7">
-        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B92" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" s="7">
         <v>0</v>
       </c>
       <c r="D92" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93" s="7">
+        <v>0</v>
+      </c>
+      <c r="C93" s="7">
+        <v>0</v>
+      </c>
+      <c r="D93" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B93" s="7">
-        <v>0</v>
-      </c>
-      <c r="C93" s="7">
-        <v>1</v>
-      </c>
-      <c r="D93" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>114</v>
+      <c r="B94" s="7">
+        <v>0</v>
+      </c>
+      <c r="C94" s="7">
+        <v>1</v>
+      </c>
+      <c r="D94" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>115</v>
+        <v>0</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>115</v>
@@ -1944,85 +1961,85 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B99" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="5"/>
-      <c r="B100" s="11" t="s">
+      <c r="B100" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="5"/>
+      <c r="B101" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C100" s="11" t="s">
+      <c r="C101" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D101" s="11" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B101" s="7">
-        <v>0</v>
-      </c>
-      <c r="C101" s="7">
-        <v>1</v>
-      </c>
-      <c r="D101" s="7">
-        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B102" s="7">
         <v>0</v>
       </c>
       <c r="C102" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D102" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B103" s="7">
+        <v>0</v>
+      </c>
+      <c r="C103" s="7">
+        <v>0</v>
+      </c>
+      <c r="D103" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B103" s="7">
-        <v>1</v>
-      </c>
-      <c r="C103" s="7">
-        <v>0</v>
-      </c>
-      <c r="D103" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B106" s="11" t="s">
-        <v>122</v>
+      <c r="B104" s="7">
+        <v>1</v>
+      </c>
+      <c r="C104" s="7">
+        <v>0</v>
+      </c>
+      <c r="D104" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>123</v>
+        <v>0</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>123</v>
@@ -2030,41 +2047,35 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B109" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="5"/>
-      <c r="B110" s="11" t="s">
+      <c r="B110" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="5"/>
+      <c r="B111" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C111" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D110" s="11" t="s">
+      <c r="D111" s="11" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B111" s="7">
-        <v>0</v>
-      </c>
-      <c r="C111" s="7">
-        <v>1</v>
-      </c>
-      <c r="D111" s="7">
-        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B112" s="7">
         <v>0</v>
@@ -2078,15 +2089,29 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B113" s="7">
+        <v>0</v>
+      </c>
+      <c r="C113" s="7">
+        <v>1</v>
+      </c>
+      <c r="D113" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B113" s="7">
-        <v>0</v>
-      </c>
-      <c r="C113" s="7">
-        <v>0</v>
-      </c>
-      <c r="D113" s="7">
+      <c r="B114" s="7">
+        <v>0</v>
+      </c>
+      <c r="C114" s="7">
+        <v>0</v>
+      </c>
+      <c r="D114" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OO-3641: add min. max. answers in csv import for QTI 2.1
Add min. and max. number of answers as options in the CSV import of
questions for QTI.21
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF45A0EF-AF9E-224E-B060-D1C5DC7DBEAA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265AB374-8265-224D-A237-D00BA17AFCBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="460" windowWidth="28320" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="137">
   <si>
     <t>Typ</t>
   </si>
@@ -427,6 +427,18 @@
   </si>
   <si>
     <t>Optional, nur in Fragenpool : Thema</t>
+  </si>
+  <si>
+    <t>Max answers</t>
+  </si>
+  <si>
+    <t>Min answers</t>
+  </si>
+  <si>
+    <t>Max. Anzahl möglicher Antworten</t>
+  </si>
+  <si>
+    <t>Min. Anzahl möglicher Antworten</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,7 +1043,7 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -1062,7 +1074,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>53</v>
       </c>
@@ -1274,7 +1286,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>87</v>
       </c>
@@ -1322,7 +1334,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>1</v>
       </c>
@@ -1336,7 +1348,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
@@ -1348,7 +1360,7 @@
       <c r="C29" s="10"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>58</v>
       </c>
@@ -1380,7 +1392,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
@@ -1442,7 +1454,7 @@
       </c>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -1460,7 +1472,7 @@
       <c r="B41" s="10"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
@@ -1471,7 +1483,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>57</v>
       </c>
@@ -1482,7 +1494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>65</v>
       </c>
@@ -1493,625 +1505,647 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="7">
+        <v>4</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="7">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B47" s="7">
         <v>3</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
-        <v>1</v>
-      </c>
-      <c r="B46" s="7" t="s">
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>1</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="5">
-        <v>1</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="5">
-        <v>1</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>-1</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>-1</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B53" s="10"/>
+    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="D53" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B55" s="10"/>
+      <c r="D55" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B54" s="10"/>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="10"/>
-      <c r="D55" s="4"/>
-    </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="10"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B57" s="10"/>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D58" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+    <row r="60" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D60" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="7">
-        <v>1</v>
-      </c>
-      <c r="D59" s="4" t="s">
+      <c r="B61" s="7">
+        <v>1</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="5">
-        <v>0</v>
-      </c>
-      <c r="B60" s="7" t="s">
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>0</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="5">
-        <v>0</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="5">
-        <v>0</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>0</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>0</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B66" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="5">
+        <v>0</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>0</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D68" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="D67" s="4" t="s">
+    <row r="69" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D69" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="11" t="s">
+    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D71" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B72" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
+    <row r="73" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B73" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D73" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B72" s="7">
-        <v>1</v>
-      </c>
-      <c r="D72" s="4" t="s">
+      <c r="B74" s="7">
+        <v>1</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
+    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B75" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B76" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
+    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B77" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D77" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
+    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B78" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D78" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="11" t="s">
+    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="5" t="s">
+    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B82" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
+    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B83" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
+    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B82" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
+      <c r="B84" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B85" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
+    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B86" s="7">
         <v>2000</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B87" s="11" t="s">
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
+    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B90" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
+    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B91" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="5" t="s">
+    <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B90" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="5"/>
-      <c r="B91" s="11" t="s">
+      <c r="B92" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="5"/>
+      <c r="B93" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C93" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D91" s="11" t="s">
+      <c r="D93" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="5" t="s">
+    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B92" s="7">
-        <v>1</v>
-      </c>
-      <c r="C92" s="7">
-        <v>0</v>
-      </c>
-      <c r="D92" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="5" t="s">
+      <c r="B94" s="7">
+        <v>1</v>
+      </c>
+      <c r="C94" s="7">
+        <v>0</v>
+      </c>
+      <c r="D94" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B93" s="7">
-        <v>0</v>
-      </c>
-      <c r="C93" s="7">
-        <v>0</v>
-      </c>
-      <c r="D93" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
+      <c r="B95" s="7">
+        <v>0</v>
+      </c>
+      <c r="C95" s="7">
+        <v>0</v>
+      </c>
+      <c r="D95" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B94" s="7">
-        <v>0</v>
-      </c>
-      <c r="C94" s="7">
-        <v>1</v>
-      </c>
-      <c r="D94" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B97" s="11" t="s">
+      <c r="B96" s="7">
+        <v>0</v>
+      </c>
+      <c r="C96" s="7">
+        <v>1</v>
+      </c>
+      <c r="D96" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
+    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B100" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="5" t="s">
+    <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="B101" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="5" t="s">
+    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B100" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="5"/>
-      <c r="B101" s="11" t="s">
+      <c r="B102" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="5"/>
+      <c r="B103" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C103" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D101" s="11" t="s">
+      <c r="D103" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
+    <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B102" s="7">
-        <v>0</v>
-      </c>
-      <c r="C102" s="7">
-        <v>1</v>
-      </c>
-      <c r="D102" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
+      <c r="B104" s="7">
+        <v>0</v>
+      </c>
+      <c r="C104" s="7">
+        <v>1</v>
+      </c>
+      <c r="D104" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B103" s="7">
-        <v>0</v>
-      </c>
-      <c r="C103" s="7">
-        <v>0</v>
-      </c>
-      <c r="D103" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="5" t="s">
+      <c r="B105" s="7">
+        <v>0</v>
+      </c>
+      <c r="C105" s="7">
+        <v>0</v>
+      </c>
+      <c r="D105" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B104" s="7">
-        <v>1</v>
-      </c>
-      <c r="C104" s="7">
-        <v>0</v>
-      </c>
-      <c r="D104" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B107" s="11" t="s">
+      <c r="B106" s="7">
+        <v>1</v>
+      </c>
+      <c r="C106" s="7">
+        <v>0</v>
+      </c>
+      <c r="D106" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="5" t="s">
+    <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="B110" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="5" t="s">
+    <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="B111" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="5" t="s">
+    <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B110" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="5"/>
-      <c r="B111" s="11" t="s">
+      <c r="B112" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="5"/>
+      <c r="B113" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C113" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D111" s="11" t="s">
+      <c r="D113" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="5" t="s">
+    <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B112" s="7">
-        <v>0</v>
-      </c>
-      <c r="C112" s="7">
-        <v>1</v>
-      </c>
-      <c r="D112" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="5" t="s">
+      <c r="B114" s="7">
+        <v>0</v>
+      </c>
+      <c r="C114" s="7">
+        <v>1</v>
+      </c>
+      <c r="D114" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B113" s="7">
-        <v>0</v>
-      </c>
-      <c r="C113" s="7">
-        <v>1</v>
-      </c>
-      <c r="D113" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="5" t="s">
+      <c r="B115" s="7">
+        <v>0</v>
+      </c>
+      <c r="C115" s="7">
+        <v>1</v>
+      </c>
+      <c r="D115" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B114" s="7">
-        <v>0</v>
-      </c>
-      <c r="C114" s="7">
-        <v>0</v>
-      </c>
-      <c r="D114" s="7">
+      <c r="B116" s="7">
+        <v>0</v>
+      </c>
+      <c r="C116" s="7">
+        <v>0</v>
+      </c>
+      <c r="D116" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OO-4438: grading time as excel import and bulk change
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Developer/Work/ws_features/OpenOLAT/src/main/resources/org/olat/ims/qti21/questionimport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265AB374-8265-224D-A237-D00BA17AFCBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12818AC-2616-E443-943E-F2067B54DF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="460" windowWidth="28320" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6920" yWindow="5600" windowWidth="28320" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="139">
   <si>
     <t>Typ</t>
   </si>
@@ -234,39 +234,12 @@
     <t>9.4.2</t>
   </si>
   <si>
-    <t>Optional, nur in Fragenpool : Schlagworte</t>
-  </si>
-  <si>
-    <t>Optional, nur in Fragenpool : Abdeckung</t>
-  </si>
-  <si>
     <t>Optional, nur in Fragenpool : Sprache</t>
   </si>
   <si>
-    <t>Optional, nur in Fragenpool : Fachbereich</t>
-  </si>
-  <si>
     <t>Optional, nur in Fragenpool : probiert ein Lizenz mit dem gleichen Key zu finden oder erstellt eine neue Freitext Lizenz</t>
   </si>
   <si>
-    <t>Optional, nur in Fragenpool : Level</t>
-  </si>
-  <si>
-    <t>Optional, nur in Fragenpool : Durchschnittliche Bearbeitungszeit, Format ist unter http://www.w3.org/TR/xmlschema-2/#duration definiert</t>
-  </si>
-  <si>
-    <t>Optional, nur in Fragenpool : Itemschwierigkeit (zwischen 0.0 und 1.0)</t>
-  </si>
-  <si>
-    <t>Optional, nur in Fragenpool : Standardabweichung Itemschwierigkeit (zwischen 0.0 und 1.0)</t>
-  </si>
-  <si>
-    <t>Optional, nur in Fragenpool : Trennschärfe (zwischen -1.0 und 1.0)</t>
-  </si>
-  <si>
-    <t>Optional, nur in Fragenpool : Anzahl Distraktoren ( 1 )</t>
-  </si>
-  <si>
     <t xml:space="preserve">Optional, nur in Fragenpool : Editor </t>
   </si>
   <si>
@@ -426,9 +399,6 @@
     <t>Grundwortschatz</t>
   </si>
   <si>
-    <t>Optional, nur in Fragenpool : Thema</t>
-  </si>
-  <si>
     <t>Max answers</t>
   </si>
   <si>
@@ -439,13 +409,49 @@
   </si>
   <si>
     <t>Min. Anzahl möglicher Antworten</t>
+  </si>
+  <si>
+    <t>Required grading time</t>
+  </si>
+  <si>
+    <t>Optional : Anzahl Distraktoren ( 1 )</t>
+  </si>
+  <si>
+    <t>Optional : Trennschärfe (zwischen -1.0 und 1.0)</t>
+  </si>
+  <si>
+    <t>Optional : Standardabweichung Itemschwierigkeit (zwischen 0.0 und 1.0)</t>
+  </si>
+  <si>
+    <t>Optional : Itemschwierigkeit (zwischen 0.0 und 1.0)</t>
+  </si>
+  <si>
+    <t>Optional : in minutes</t>
+  </si>
+  <si>
+    <t>Optional : Durchschnittliche Bearbeitungszeit, Format ist unter http://www.w3.org/TR/xmlschema-2/#duration definiert</t>
+  </si>
+  <si>
+    <t>Optional : Level</t>
+  </si>
+  <si>
+    <t>Optional : Fachbereich</t>
+  </si>
+  <si>
+    <t>Optional : Abdeckung</t>
+  </si>
+  <si>
+    <t>Optional : Schlagworte</t>
+  </si>
+  <si>
+    <t>Optional : Thema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -525,6 +531,14 @@
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -608,7 +622,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -644,6 +658,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="16" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1028,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,12 +1081,12 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="A3" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" s="1"/>
@@ -1083,7 +1100,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,19 +1115,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
@@ -1119,17 +1136,17 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="4" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1141,10 +1158,10 @@
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -1153,7 +1170,7 @@
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -1165,10 +1182,10 @@
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -1177,376 +1194,377 @@
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
       <c r="D14" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>51</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>127</v>
       </c>
       <c r="B15" s="8">
-        <v>0.55000000000000004</v>
+        <v>5</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="8">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="4" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="8">
-        <v>-0.33</v>
+        <v>0.6</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="8">
-        <v>1</v>
+        <v>-0.33</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="4" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>67</v>
+        <v>78</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="7">
-        <v>1</v>
+      <c r="A25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="4" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>6</v>
+        <v>59</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
-        <v>1</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="7" t="s">
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="D29" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>10</v>
+      <c r="B31" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="7">
-        <v>5</v>
+        <v>57</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="7">
         <v>5</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
-        <v>1</v>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
-        <v>1</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="7"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>1</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
-        <v>1</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="7"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>1</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B40" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="10"/>
+      <c r="C40" s="7"/>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="10"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>35</v>
-      </c>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="10"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B44" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+    <row r="45" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" s="7">
-        <v>4</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B46" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="7">
+        <v>2</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B48" s="7">
         <v>3</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="5">
-        <v>1</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1554,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>21</v>
@@ -1565,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>21</v>
@@ -1573,13 +1591,13 @@
     </row>
     <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1587,7 +1605,7 @@
         <v>-1</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>25</v>
@@ -1598,7 +1616,7 @@
         <v>-1</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>25</v>
@@ -1609,79 +1627,79 @@
         <v>-1</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B55" s="10"/>
+    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D55" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B56" s="10"/>
+      <c r="D56" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="10"/>
-      <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B57" s="10"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>37</v>
-      </c>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="10"/>
+      <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D60" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
+    <row r="61" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D60" s="4" t="s">
+      <c r="B61" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="7">
-        <v>1</v>
-      </c>
-      <c r="D61" s="4" t="s">
+      <c r="B62" s="7">
+        <v>1</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="5">
-        <v>0</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1689,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>42</v>
@@ -1700,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>42</v>
@@ -1711,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>42</v>
@@ -1719,24 +1737,24 @@
     </row>
     <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1744,89 +1762,89 @@
         <v>0</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="5">
+        <v>0</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D69" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D70" s="4" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D72" s="4" t="s">
+      <c r="B73" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
+    <row r="74" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D73" s="4" t="s">
+      <c r="B74" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B74" s="7">
-        <v>1</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>20</v>
+        <v>59</v>
+      </c>
+      <c r="B75" s="7">
+        <v>1</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>95</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>42</v>
@@ -1834,296 +1852,293 @@
     </row>
     <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>104</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B84" s="7">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="B85" s="7">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B86" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B87" s="7">
         <v>2000</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>113</v>
+        <v>0</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B92" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="5"/>
-      <c r="B93" s="11" t="s">
+      <c r="B93" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="5"/>
+      <c r="B94" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C94" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="D94" s="11" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B94" s="7">
-        <v>1</v>
-      </c>
-      <c r="C94" s="7">
-        <v>0</v>
-      </c>
-      <c r="D94" s="7">
-        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B95" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95" s="7">
         <v>0</v>
       </c>
       <c r="D95" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B96" s="7">
         <v>0</v>
       </c>
       <c r="C96" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B99" s="11" t="s">
-        <v>114</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B97" s="7">
+        <v>0</v>
+      </c>
+      <c r="C97" s="7">
+        <v>1</v>
+      </c>
+      <c r="D97" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>115</v>
+        <v>0</v>
+      </c>
+      <c r="B100" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B102" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="5"/>
-      <c r="B103" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C103" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D103" s="11" t="s">
-        <v>119</v>
+      <c r="B103" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B104" s="7">
-        <v>0</v>
-      </c>
-      <c r="C104" s="7">
-        <v>1</v>
-      </c>
-      <c r="D104" s="7">
-        <v>0</v>
+      <c r="A104" s="5"/>
+      <c r="B104" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B105" s="7">
         <v>0</v>
       </c>
       <c r="C105" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D105" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B106" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C106" s="7">
         <v>0</v>
       </c>
       <c r="D106" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B109" s="11" t="s">
-        <v>122</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" s="7">
+        <v>1</v>
+      </c>
+      <c r="C107" s="7">
+        <v>0</v>
+      </c>
+      <c r="D107" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>123</v>
+        <v>0</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B112" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="5"/>
-      <c r="B113" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C113" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D113" s="11" t="s">
-        <v>126</v>
+      <c r="B113" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B114" s="7">
-        <v>0</v>
-      </c>
-      <c r="C114" s="7">
-        <v>1</v>
-      </c>
-      <c r="D114" s="7">
-        <v>0</v>
+      <c r="A114" s="5"/>
+      <c r="B114" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B115" s="7">
         <v>0</v>
@@ -2137,15 +2152,29 @@
     </row>
     <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B116" s="7">
         <v>0</v>
       </c>
       <c r="C116" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D116" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B117" s="7">
+        <v>0</v>
+      </c>
+      <c r="C117" s="7">
+        <v>0</v>
+      </c>
+      <c r="D117" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OO-4969: don't ask length of text entry, it's not used in excel import
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Developer/Work/ws_features/OpenOLAT/src/main/resources/org/olat/ims/qti21/questionimport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Developer/Work/ws_branches/OpenOLAT/src/main/resources/org/olat/ims/qti21/questionimport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12818AC-2616-E443-943E-F2067B54DF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6441F8-462E-1845-904D-950669B1D045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="5600" windowWidth="28320" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="3460" windowWidth="28320" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
   <si>
     <t>Typ</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Ein Text element</t>
   </si>
   <si>
-    <t>20,50</t>
-  </si>
-  <si>
     <t>Es können beliebig viele Text und Lückenelemente aufgelistet werden. Die Leerzeile markiert das Ende des Frageitems. Die nächste Zeile sollte wieder mit „Typ“ beginnen und markiert den Beginn des nächsten Frageitems.</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>,</t>
   </si>
   <si>
-    <t>2,2</t>
-  </si>
-  <si>
     <t>dass das Wetter</t>
   </si>
   <si>
@@ -258,9 +252,6 @@
     <t>verbannen;Verbot</t>
   </si>
   <si>
-    <t>Eine Lücke, Länge 20, Anzahl Zeichen 50. Wenn richtig gibt’s einen Punkt. Strickpunkt trennt Synonyme bzw. mehrere korrekte Lösungen</t>
-  </si>
-  <si>
     <t>Feedback correct answer</t>
   </si>
   <si>
@@ -445,6 +436,9 @@
   </si>
   <si>
     <t>Optional : Thema</t>
+  </si>
+  <si>
+    <t>Eine Lücke, Länge 20. Wenn richtig gibt’s einen Punkt. Strickpunkt trennt Synonyme bzw. mehrere korrekte Lösungen</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,16 +1056,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1082,7 +1076,7 @@
     </row>
     <row r="3" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -1093,19 +1087,19 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -1117,231 +1111,231 @@
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
       <c r="D14" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B15" s="8">
         <v>5</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="8">
         <v>0.55000000000000004</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="8">
         <v>0.6</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="8">
         <v>-0.33</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="8">
         <v>1</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="7">
         <v>1</v>
@@ -1368,20 +1362,20 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="C28" s="7">
+        <v>20</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1391,29 +1385,29 @@
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="7">
         <v>5</v>
@@ -1426,20 +1420,20 @@
         <v>5</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2</v>
       </c>
       <c r="D35" s="4"/>
     </row>
@@ -1448,7 +1442,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="4"/>
@@ -1458,8 +1452,8 @@
         <v>1</v>
       </c>
       <c r="B37" s="7"/>
-      <c r="C37" s="7" t="s">
-        <v>13</v>
+      <c r="C37" s="7">
+        <v>2</v>
       </c>
       <c r="D37" s="4"/>
     </row>
@@ -1468,18 +1462,18 @@
         <v>5</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>1</v>
       </c>
       <c r="B39" s="7"/>
-      <c r="C39" s="7" t="s">
-        <v>13</v>
+      <c r="C39" s="7">
+        <v>2</v>
       </c>
       <c r="D39" s="4"/>
     </row>
@@ -1488,7 +1482,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="4"/>
@@ -1506,18 +1500,18 @@
         <v>0</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>3</v>
@@ -1525,40 +1519,40 @@
     </row>
     <row r="45" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B46" s="7">
         <v>4</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B47" s="7">
         <v>2</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B48" s="7">
         <v>3</v>
@@ -1572,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1583,10 +1577,10 @@
         <v>1</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1594,10 +1588,10 @@
         <v>1</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1605,10 +1599,10 @@
         <v>-1</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1616,10 +1610,10 @@
         <v>-1</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1627,10 +1621,10 @@
         <v>-1</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1638,16 +1632,16 @@
         <v>-1</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B56" s="10"/>
       <c r="D56" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1663,18 +1657,18 @@
         <v>0</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>3</v>
@@ -1682,18 +1676,18 @@
     </row>
     <row r="61" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B62" s="7">
         <v>1</v>
@@ -1707,10 +1701,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1718,10 +1712,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1729,10 +1723,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1740,10 +1734,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1751,10 +1745,10 @@
         <v>1</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1762,10 +1756,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1773,15 +1767,15 @@
         <v>0</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D70" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1789,18 +1783,18 @@
         <v>0</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>3</v>
@@ -1808,18 +1802,18 @@
     </row>
     <row r="74" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B75" s="7">
         <v>1</v>
@@ -1830,46 +1824,46 @@
     </row>
     <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1877,28 +1871,28 @@
         <v>0</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B85" s="7">
         <v>1</v>
@@ -1906,7 +1900,7 @@
     </row>
     <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B86" s="7">
         <v>200</v>
@@ -1914,7 +1908,7 @@
     </row>
     <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B87" s="7">
         <v>2000</v>
@@ -1925,28 +1919,28 @@
         <v>0</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B93" s="7">
         <v>1</v>
@@ -1955,18 +1949,18 @@
     <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
       <c r="B94" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B95" s="7">
         <v>1</v>
@@ -1980,7 +1974,7 @@
     </row>
     <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B96" s="7">
         <v>0</v>
@@ -1994,7 +1988,7 @@
     </row>
     <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B97" s="7">
         <v>0</v>
@@ -2011,28 +2005,28 @@
         <v>0</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B103" s="7">
         <v>1</v>
@@ -2041,18 +2035,18 @@
     <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="5"/>
       <c r="B104" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D104" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B105" s="7">
         <v>0</v>
@@ -2066,7 +2060,7 @@
     </row>
     <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B106" s="7">
         <v>0</v>
@@ -2080,7 +2074,7 @@
     </row>
     <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B107" s="7">
         <v>1</v>
@@ -2097,28 +2091,28 @@
         <v>0</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B113" s="7">
         <v>1</v>
@@ -2127,18 +2121,18 @@
     <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="5"/>
       <c r="B114" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B115" s="7">
         <v>0</v>
@@ -2152,7 +2146,7 @@
     </row>
     <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B116" s="7">
         <v>0</v>
@@ -2166,7 +2160,7 @@
     </row>
     <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B117" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
OO-5573: CSV import of numerical questions
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Developer/Work/ws_branches/OpenOLAT/src/main/resources/org/olat/ims/qti21/questionimport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6441F8-462E-1845-904D-950669B1D045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD923F6-DF86-A74A-A83C-7E34DD73DE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="3460" windowWidth="28320" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15460" yWindow="500" windowWidth="31960" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="149">
   <si>
     <t>Typ</t>
   </si>
@@ -439,6 +439,42 @@
   </si>
   <si>
     <t>Eine Lücke, Länge 20. Wenn richtig gibt’s einen Punkt. Strickpunkt trennt Synonyme bzw. mehrere korrekte Lösungen</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>Die Lösung entspricht exakt der eingegebenen Lösung</t>
+  </si>
+  <si>
+    <t>21 + 21?</t>
+  </si>
+  <si>
+    <t>Quadratwurzel von 2</t>
+  </si>
+  <si>
+    <t>1.41;1.40;1.42</t>
+  </si>
+  <si>
+    <t>absolute</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>Die Lösung ist 1.41, dann die untere Schranke 1.40 und die obere Schranke 1.42. Alle Lösungen zwischen 1.40 und 1.42 sind gültig.</t>
+  </si>
+  <si>
+    <t>20;10;10</t>
+  </si>
+  <si>
+    <t>12.78 + 7.22?</t>
+  </si>
+  <si>
+    <t>Die Lösung ist 20, dann die relative untere Schranke 10 Procent und die obere Schranke 10 Procent. Alle Lösungen zwischen 18 und 22 sind gültig, denn die untere Schranke bedeutet minus 10% (20-2) und die obere Schranke plus 10% (20+2).</t>
+  </si>
+  <si>
+    <t>Quadratwurzel und Addition</t>
   </si>
 </sst>
 </file>
@@ -1039,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1497,13 +1533,14 @@
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>33</v>
+        <v>56</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1511,359 +1548,376 @@
         <v>55</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B46" s="7">
-        <v>4</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>122</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
-        <v>121</v>
+      <c r="A47" s="5">
+        <v>1</v>
       </c>
       <c r="B47" s="7">
-        <v>2</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C47" s="7"/>
       <c r="D47" s="4" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>1</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>1</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="10"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="7">
+        <v>4</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="7">
+        <v>2</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B58" s="7">
         <v>3</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="5">
-        <v>1</v>
-      </c>
-      <c r="B49" s="7" t="s">
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
+        <v>1</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="5">
-        <v>1</v>
-      </c>
-      <c r="B50" s="7" t="s">
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>1</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D60" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="5">
-        <v>1</v>
-      </c>
-      <c r="B51" s="7" t="s">
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
+        <v>1</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="5">
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
         <v>-1</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="5">
-        <v>-1</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="5">
-        <v>-1</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="5">
-        <v>-1</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B56" s="10"/>
-      <c r="D56" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B57" s="10"/>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="10"/>
-      <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B62" s="7">
-        <v>1</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="5">
-        <v>0</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B66" s="10"/>
       <c r="D66" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="5">
-        <v>1</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="5">
-        <v>0</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="10"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="10"/>
+      <c r="D68" s="4"/>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="5">
-        <v>0</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="D70" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="B72" s="7">
+        <v>1</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
-        <v>55</v>
+      <c r="A73" s="5">
+        <v>0</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
-        <v>63</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>0</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B75" s="7">
-        <v>1</v>
+      <c r="A75" s="5">
+        <v>0</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
-        <v>81</v>
+      <c r="A76" s="5">
+        <v>0</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
-        <v>82</v>
+      <c r="A77" s="5">
+        <v>1</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
-        <v>82</v>
+      <c r="A78" s="5">
+        <v>0</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
-        <v>81</v>
+      <c r="A79" s="5">
+        <v>0</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>83</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D80" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1871,7 +1925,10 @@
         <v>0</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>92</v>
+        <v>79</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1879,15 +1936,21 @@
         <v>55</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1897,107 +1960,100 @@
       <c r="B85" s="7">
         <v>1</v>
       </c>
+      <c r="D85" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B86" s="7">
-        <v>200</v>
+        <v>81</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B87" s="7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>101</v>
+        <v>82</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>101</v>
+        <v>0</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B93" s="7">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="5"/>
-      <c r="B94" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>22</v>
+      <c r="A94" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="B95" s="7">
         <v>1</v>
-      </c>
-      <c r="C95" s="7">
-        <v>0</v>
-      </c>
-      <c r="D95" s="7">
-        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B96" s="7">
-        <v>0</v>
-      </c>
-      <c r="C96" s="7">
-        <v>0</v>
-      </c>
-      <c r="D96" s="7">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B97" s="7">
-        <v>0</v>
-      </c>
-      <c r="C97" s="7">
-        <v>1</v>
-      </c>
-      <c r="D97" s="7">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2005,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2013,7 +2069,7 @@
         <v>55</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2021,7 +2077,7 @@
         <v>63</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2035,24 +2091,24 @@
     <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="5"/>
       <c r="B104" s="11" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B105" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D105" s="7">
         <v>0</v>
@@ -2060,7 +2116,7 @@
     </row>
     <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B106" s="7">
         <v>0</v>
@@ -2074,13 +2130,13 @@
     </row>
     <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B107" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107" s="7">
         <v>0</v>
@@ -2091,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2099,7 +2155,7 @@
         <v>55</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2107,7 +2163,7 @@
         <v>63</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2121,18 +2177,18 @@
     <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="5"/>
       <c r="B114" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B115" s="7">
         <v>0</v>
@@ -2146,29 +2202,115 @@
     </row>
     <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B116" s="7">
         <v>0</v>
       </c>
       <c r="C116" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D116" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B117" s="7">
+        <v>1</v>
+      </c>
+      <c r="C117" s="7">
+        <v>0</v>
+      </c>
+      <c r="D117" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B123" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="5"/>
+      <c r="B124" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B125" s="7">
+        <v>0</v>
+      </c>
+      <c r="C125" s="7">
+        <v>1</v>
+      </c>
+      <c r="D125" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B126" s="7">
+        <v>0</v>
+      </c>
+      <c r="C126" s="7">
+        <v>1</v>
+      </c>
+      <c r="D126" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B117" s="7">
-        <v>0</v>
-      </c>
-      <c r="C117" s="7">
-        <v>0</v>
-      </c>
-      <c r="D117" s="7">
+      <c r="B127" s="7">
+        <v>0</v>
+      </c>
+      <c r="C127" s="7">
+        <v>0</v>
+      </c>
+      <c r="D127" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OO-6270: add example of CSV import for inline choice
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD923F6-DF86-A74A-A83C-7E34DD73DE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AACAD9-9393-A741-8757-B4DF1E92B210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15460" yWindow="500" windowWidth="31960" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="500" windowWidth="31960" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="164">
   <si>
     <t>Typ</t>
   </si>
@@ -129,9 +129,6 @@
     <t>MC</t>
   </si>
   <si>
-    <t>Fragetpy: Multiple Choice</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
@@ -475,6 +472,54 @@
   </si>
   <si>
     <t>Quadratwurzel und Addition</t>
+  </si>
+  <si>
+    <t>Inlinechoice</t>
+  </si>
+  <si>
+    <t>Hansel und Gretel</t>
+  </si>
+  <si>
+    <t>Eine lange Geschichte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vor einem grossen Walde wohnte ein armer </t>
+  </si>
+  <si>
+    <t>|.|;|!</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>Holzhacker mit seiner Frau und seinen zwei Kindern</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>das Bubchen hiesst Hansel und das Madchen Gretel</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Er hatte wenig zu beissen und zu brechen</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Fragetyp: Multiple Choice</t>
+  </si>
+  <si>
+    <t>Fragetyp: Inline choice oder Lückentext mit Dropdown</t>
+  </si>
+  <si>
+    <t>Ein Dropdown. Wenn richtig gibt’s einen Punkt. Strichpunkt trennt die Antwortmöglichkeiten per Default aber hier wird / als Separator definirt. Richtige Antwort ist hier leer.</t>
+  </si>
+  <si>
+    <t>Ein Dropdown. Wenn richtig gibt’s einen Punkt. Strichpunkt trennt die Antwortmöglichkeiten per Default aber hier wird / als Separator definirt. Richtige Antwort ist hier Strichpunk.</t>
   </si>
 </sst>
 </file>
@@ -526,6 +571,7 @@
       <sz val="12"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -541,18 +587,21 @@
       <sz val="12"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -561,6 +610,7 @@
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -572,7 +622,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,8 +634,14 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -605,6 +661,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -652,7 +723,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -694,6 +765,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1075,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,8 +1172,9 @@
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="91.33203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="90.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="84.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1112,7 +1199,7 @@
     </row>
     <row r="3" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -1123,19 +1210,19 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -1147,231 +1234,231 @@
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
       <c r="D14" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B15" s="8">
         <v>5</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="8">
         <v>0.55000000000000004</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="8">
         <v>0.6</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="8">
         <v>-0.33</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="8">
         <v>1</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="7">
         <v>1</v>
@@ -1398,13 +1485,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="7">
         <v>20</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1421,19 +1508,19 @@
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>9</v>
@@ -1443,7 +1530,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" s="7">
         <v>5</v>
@@ -1533,29 +1620,29 @@
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B45" s="7">
         <v>3</v>
@@ -1568,7 +1655,7 @@
         <v>5</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="4"/>
@@ -1582,7 +1669,7 @@
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1590,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="4"/>
@@ -1600,13 +1687,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>142</v>
-      </c>
       <c r="D49" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1614,7 +1701,7 @@
         <v>5</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="4"/>
@@ -1624,13 +1711,13 @@
         <v>1</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1645,12 +1732,12 @@
         <v>32</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>33</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>15</v>
@@ -1661,7 +1748,7 @@
     </row>
     <row r="55" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>16</v>
@@ -1672,29 +1759,29 @@
     </row>
     <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B56" s="7">
         <v>4</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B57" s="7">
         <v>2</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="7">
         <v>3</v>
@@ -1769,7 +1856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>-1</v>
       </c>
@@ -1780,443 +1867,484 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B66" s="10"/>
       <c r="D66" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B67" s="10"/>
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B68" s="10"/>
-      <c r="D68" s="4"/>
-    </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="11" t="s">
+    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C68" s="16"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="16"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" s="16"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B71" s="17">
+        <v>4</v>
+      </c>
+      <c r="C71" s="16"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="16"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" s="15">
+        <v>1</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A74" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="16"/>
+      <c r="D74" s="19"/>
+    </row>
+    <row r="75" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="15">
+        <v>1</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A76" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="16"/>
+      <c r="D76" s="19"/>
+    </row>
+    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="15">
+        <v>1</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A78" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="16"/>
+      <c r="D78" s="19"/>
+    </row>
+    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="15">
+        <v>1</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B80" s="10"/>
+      <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D81" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B72" s="7">
-        <v>1</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="5">
-        <v>0</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="5">
-        <v>0</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="5">
-        <v>0</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="5">
-        <v>0</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="5">
-        <v>1</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="5">
-        <v>0</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="5">
-        <v>0</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D80" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>86</v>
+        <v>56</v>
+      </c>
+      <c r="B84" s="7">
+        <v>1</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B85" s="7">
-        <v>1</v>
+      <c r="A85" s="5">
+        <v>0</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="5" t="s">
-        <v>81</v>
+      <c r="A86" s="5">
+        <v>0</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
-        <v>82</v>
+      <c r="A87" s="5">
+        <v>0</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D87" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
+        <v>0</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="5">
+        <v>1</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>93</v>
+    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
+        <v>0</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>0</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D92" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>94</v>
+        <v>0</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B95" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B96" s="7">
-        <v>200</v>
+        <v>62</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="B97" s="7">
-        <v>2000</v>
+        <v>1</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B100" s="11" t="s">
-        <v>97</v>
+        <v>81</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B103" s="7">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="5"/>
+      <c r="A104" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="B104" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B105" s="7">
-        <v>1</v>
-      </c>
-      <c r="C105" s="7">
-        <v>0</v>
-      </c>
-      <c r="D105" s="7">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B106" s="7">
-        <v>0</v>
-      </c>
-      <c r="C106" s="7">
-        <v>0</v>
-      </c>
-      <c r="D106" s="7">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="B107" s="7">
-        <v>0</v>
-      </c>
-      <c r="C107" s="7">
-        <v>1</v>
-      </c>
-      <c r="D107" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B110" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>103</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B108" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B109" s="7">
+        <v>2000</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>103</v>
+        <v>0</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B113" s="7">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="5"/>
-      <c r="B114" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C114" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D114" s="11" t="s">
-        <v>107</v>
+      <c r="A114" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="B115" s="7">
-        <v>0</v>
-      </c>
-      <c r="C115" s="7">
-        <v>1</v>
-      </c>
-      <c r="D115" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B116" s="7">
-        <v>0</v>
-      </c>
-      <c r="C116" s="7">
-        <v>0</v>
-      </c>
-      <c r="D116" s="7">
-        <v>1</v>
+      <c r="A116" s="5"/>
+      <c r="B116" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C116" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D116" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B117" s="7">
         <v>1</v>
@@ -2228,89 +2356,203 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B120" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>111</v>
+    <row r="118" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B118" s="7">
+        <v>0</v>
+      </c>
+      <c r="C118" s="7">
+        <v>0</v>
+      </c>
+      <c r="D118" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B119" s="7">
+        <v>0</v>
+      </c>
+      <c r="C119" s="7">
+        <v>1</v>
+      </c>
+      <c r="D119" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B122" s="7" t="s">
-        <v>111</v>
+        <v>0</v>
+      </c>
+      <c r="B122" s="11" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B123" s="7">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="5"/>
-      <c r="B124" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C124" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D124" s="11" t="s">
-        <v>114</v>
+      <c r="A124" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
-        <v>115</v>
+        <v>56</v>
       </c>
       <c r="B125" s="7">
-        <v>0</v>
-      </c>
-      <c r="C125" s="7">
-        <v>1</v>
-      </c>
-      <c r="D125" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B126" s="7">
-        <v>0</v>
-      </c>
-      <c r="C126" s="7">
-        <v>1</v>
-      </c>
-      <c r="D126" s="7">
-        <v>0</v>
+      <c r="A126" s="5"/>
+      <c r="B126" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D126" s="11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B127" s="7">
         <v>0</v>
       </c>
       <c r="C127" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D127" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B128" s="7">
+        <v>0</v>
+      </c>
+      <c r="C128" s="7">
+        <v>0</v>
+      </c>
+      <c r="D128" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B129" s="7">
+        <v>1</v>
+      </c>
+      <c r="C129" s="7">
+        <v>0</v>
+      </c>
+      <c r="D129" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A134" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A135" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B135" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A136" s="5"/>
+      <c r="B136" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C136" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D136" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A137" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B137" s="7">
+        <v>0</v>
+      </c>
+      <c r="C137" s="7">
+        <v>1</v>
+      </c>
+      <c r="D137" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A138" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B138" s="7">
+        <v>0</v>
+      </c>
+      <c r="C138" s="7">
+        <v>1</v>
+      </c>
+      <c r="D138" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A139" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B139" s="7">
+        <v>0</v>
+      </c>
+      <c r="C139" s="7">
+        <v>0</v>
+      </c>
+      <c r="D139" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>